<commit_message>
nombre personas y cirugias
</commit_message>
<xml_diff>
--- a/pandas_multiple.xlsx
+++ b/pandas_multiple.xlsx
@@ -402,7 +402,7 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>21</v>
+        <v>4963596</v>
       </c>
       <c r="C2">
         <v>31</v>
@@ -413,7 +413,7 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>22</v>
+        <v>4963596</v>
       </c>
       <c r="C3">
         <v>32</v>
@@ -424,7 +424,7 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>23</v>
+        <v>4963596</v>
       </c>
       <c r="C4">
         <v>33</v>
@@ -435,7 +435,7 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>24</v>
+        <v>4963596</v>
       </c>
       <c r="C5">
         <v>34</v>

</xml_diff>